<commit_message>
Enchacement in duplication Check
</commit_message>
<xml_diff>
--- a/wwwroot/UploadExcelFile/Customer.xlsx
+++ b/wwwroot/UploadExcelFile/Customer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaddiAbhilash\OneDrive - Anthology Inc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://anthologyinc-my.sharepoint.com/personal/abhilashm_anthology_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE21B25B-2C7A-48D7-9E73-121D0E918DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{9D55D45E-F004-4F25-81D3-776FE566EF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{739A5571-9C57-44BA-8464-61658F6D8EBD}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" xr2:uid="{496FBD46-72D2-4406-ABBB-D1A8C774D99B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{496FBD46-72D2-4406-ABBB-D1A8C774D99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>FirstName</t>
   </si>
@@ -71,26 +71,26 @@
     <t>Bangalore</t>
   </si>
   <si>
-    <t>A@gmail.com</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
     <t>30-02-1998</t>
   </si>
   <si>
-    <t>Santhosh</t>
-  </si>
-  <si>
-    <t>R</t>
+    <t xml:space="preserve">A@gmail.com	</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Divyaaa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +113,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -142,13 +148,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -165,6 +173,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D5E940-7824-4215-9436-8C876781A49E}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,6 +488,7 @@
     <col min="2" max="2" width="16.36328125" customWidth="1"/>
     <col min="3" max="3" width="13.453125" customWidth="1"/>
     <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" customWidth="1"/>
     <col min="10" max="10" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -513,75 +526,42 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4">
+        <v>12121</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
-        <v>212121</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>104</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>212121</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{A214C1BE-748F-467C-BF09-04436DBDDEAF}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{E70850C4-5DD7-4C64-A720-D9501E54F997}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{6B9A06AD-383D-49E4-8AB2-EE99FDF05251}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>